<commit_message>
Validation updates + tests
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9084"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Lying on back</t>
   </si>
@@ -60,9 +60,6 @@
     <t>standing lift stretched arms</t>
   </si>
   <si>
-    <t>Is not used in the validation pdf and the model is incorrect positioned</t>
-  </si>
-  <si>
     <t>Position AMS</t>
   </si>
   <si>
@@ -93,7 +90,28 @@
     <t>Fig 3e - held away about 60 cm</t>
   </si>
   <si>
-    <t>?</t>
+    <t>percent error min</t>
+  </si>
+  <si>
+    <t>percent error max</t>
+  </si>
+  <si>
+    <t>Flexed actively foward?</t>
+  </si>
+  <si>
+    <t>% min error</t>
+  </si>
+  <si>
+    <t>% max error</t>
+  </si>
+  <si>
+    <t>optimal % min error</t>
+  </si>
+  <si>
+    <t>optimal % max error</t>
+  </si>
+  <si>
+    <t>The photo shows that the elbows are resting on the legs, which is unknown forces.</t>
   </si>
 </sst>
 </file>
@@ -124,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,18 +152,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,7 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -171,20 +177,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,6 +225,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>Wilke validation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -280,34 +326,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Ark1'!$B$2:$B$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Ark1'!$B$2:$B$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Ark1'!$B$2,'Ark1'!$B$4:$B$10)</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Lying on back</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seating flexed no support</c:v>
+                  <c:v>seating relaxed</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seating relaxed</c:v>
+                  <c:v>Seating strait no support</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Seating strait no support</c:v>
+                  <c:v>standing</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>standing</c:v>
+                  <c:v>standing flexed</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>standing flexed</c:v>
+                  <c:v>standing lift close</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>standing lift close</c:v>
+                  <c:v>standing lift flexed</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>standing lift flexed</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>standing lift stretched arms</c:v>
                 </c:pt>
               </c:strCache>
@@ -315,43 +365,47 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$D$2:$D$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Ark1'!$D$2:$D$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Ark1'!$D$2,'Ark1'!$D$4:$D$10)</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.24546952224052718</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.64415156507413507</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64415156507413507</c:v>
+                  <c:v>1.1976935749588138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7051070840197694</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.1054365733113674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7841845140032948</c:v>
+                  <c:v>2.0955518945634268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8879736408566723</c:v>
+                  <c:v>4.6457990115321248</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2009884678747937</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.3426688632619443</c:v>
+                  <c:v>3.4514003294892914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E1CF-406B-BF89-2A40E0630499}"/>
+              <c16:uniqueId val="{00000000-58E2-4F83-9F7E-5C46D490A0AB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -381,34 +435,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Ark1'!$B$2:$B$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Ark1'!$B$2:$B$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Ark1'!$B$2,'Ark1'!$B$4:$B$10)</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Lying on back</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seating flexed no support</c:v>
+                  <c:v>seating relaxed</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seating relaxed</c:v>
+                  <c:v>Seating strait no support</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Seating strait no support</c:v>
+                  <c:v>standing</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>standing</c:v>
+                  <c:v>standing flexed</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>standing flexed</c:v>
+                  <c:v>standing lift close</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>standing lift close</c:v>
+                  <c:v>standing lift flexed</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>standing lift flexed</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>standing lift stretched arms</c:v>
                 </c:pt>
               </c:strCache>
@@ -416,35 +474,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$F$2:$F$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Ark1'!$F$2:$F$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Ark1'!$F$2,'Ark1'!$F$4:$F$10)</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>3.6</c:v>
                 </c:pt>
               </c:numCache>
@@ -452,7 +514,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E1CF-406B-BF89-2A40E0630499}"/>
+              <c16:uniqueId val="{00000001-58E2-4F83-9F7E-5C46D490A0AB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -465,12 +527,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1572002656"/>
-        <c:axId val="1567407792"/>
+        <c:axId val="53381760"/>
+        <c:axId val="61739680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1572002656"/>
+        <c:axId val="53381760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,7 +574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1567407792"/>
+        <c:crossAx val="61739680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -521,7 +582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1567407792"/>
+        <c:axId val="61739680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1572002656"/>
+        <c:crossAx val="53381760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1200,15 +1261,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1499,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,16 +1574,18 @@
     <col min="4" max="4" width="9.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="3"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1536,11 +1599,22 @@
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1559,33 +1633,67 @@
         <f>E2/E6</f>
         <v>0.2</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="G2" s="9">
+        <f>C2*C31</f>
+        <v>141.54999999999998</v>
+      </c>
+      <c r="H2" s="10">
+        <f>C2*C32</f>
+        <v>156.45000000000002</v>
+      </c>
+      <c r="I2" s="14">
+        <f>(C6*F2)*C31</f>
+        <v>115.33</v>
+      </c>
+      <c r="J2" s="14">
+        <f>(D6*G2)*C32</f>
+        <v>148.6275</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
       <c r="D3" s="5">
         <f>C3/C6</f>
         <v>0</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>0.9</v>
+      </c>
       <c r="F3" s="5">
         <f>E3/E6</f>
+        <v>1.8</v>
+      </c>
+      <c r="G3" s="11">
+        <f>C3*C31</f>
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="17">
+        <f>C3*C32</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <f>(C6*F3)*C31</f>
+        <v>1037.97</v>
+      </c>
+      <c r="J3" s="11">
+        <f>(C6*F3)*C32</f>
+        <v>1147.2300000000002</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1604,21 +1712,36 @@
         <f>E4/E6</f>
         <v>0.54</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="G4" s="9">
+        <f>C4*C31</f>
+        <v>371.45</v>
+      </c>
+      <c r="H4" s="10">
+        <f>C4*C32</f>
+        <v>410.55</v>
+      </c>
+      <c r="I4" s="14">
+        <f>(C6*F4)*C31</f>
+        <v>311.39100000000002</v>
+      </c>
+      <c r="J4" s="14">
+        <f>(C6*F4)*C32</f>
+        <v>344.16900000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8">
-        <v>428</v>
+      <c r="C5" s="7">
+        <v>727</v>
       </c>
       <c r="D5" s="3">
         <f>C5/C6</f>
-        <v>0.7051070840197694</v>
+        <v>1.1976935749588138</v>
       </c>
       <c r="E5">
         <v>0.45</v>
@@ -1627,11 +1750,26 @@
         <f>E5/E6</f>
         <v>0.9</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="G5" s="9">
+        <f>C5*C31</f>
+        <v>690.65</v>
+      </c>
+      <c r="H5" s="10">
+        <f>C5*C32</f>
+        <v>763.35</v>
+      </c>
+      <c r="I5" s="14">
+        <f>(C6*F5)*C31</f>
+        <v>518.98500000000001</v>
+      </c>
+      <c r="J5" s="14">
+        <f>(C6*F5)*C32</f>
+        <v>573.61500000000012</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1650,22 +1788,36 @@
         <f>E6/E6</f>
         <v>1</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="9">
+        <f>C6*C31</f>
+        <v>576.65</v>
+      </c>
+      <c r="H6" s="10">
+        <f>C6*C32</f>
+        <v>637.35</v>
+      </c>
+      <c r="I6" s="14">
+        <f>(C6*F6)*C31</f>
+        <v>576.65</v>
+      </c>
+      <c r="J6" s="14">
+        <f>(C6*F6)*C32</f>
+        <v>637.35</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8">
-        <v>1083</v>
+      <c r="C7" s="7">
+        <v>1278</v>
       </c>
       <c r="D7" s="3">
         <f>C7/C6</f>
-        <v>1.7841845140032948</v>
+        <v>2.1054365733113674</v>
       </c>
       <c r="E7">
         <v>1.1000000000000001</v>
@@ -1674,76 +1826,155 @@
         <f>E7/E6</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="G7" s="9">
+        <f>C7*C31</f>
+        <v>1214.0999999999999</v>
+      </c>
+      <c r="H7" s="10">
+        <f>C7*C32</f>
+        <v>1341.9</v>
+      </c>
+      <c r="I7" s="14">
+        <f>(C6*F7)*C31</f>
+        <v>1268.6300000000001</v>
+      </c>
+      <c r="J7" s="14">
+        <f>(C6*F7)*C32</f>
+        <v>1402.17</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10">
-        <v>1753</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="15">
+        <v>1272</v>
+      </c>
+      <c r="D8" s="16">
         <f>C8/C6</f>
-        <v>2.8879736408566723</v>
-      </c>
-      <c r="E8" s="9">
+        <v>2.0955518945634268</v>
+      </c>
+      <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="16">
         <f>E8/E6</f>
         <v>2</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="G8" s="9">
+        <f>C8*C31</f>
+        <v>1208.3999999999999</v>
+      </c>
+      <c r="H8" s="13">
+        <f>C8*C32</f>
+        <v>1335.6000000000001</v>
+      </c>
+      <c r="I8" s="14">
+        <f>(C6*F8)*C31</f>
+        <v>1153.3</v>
+      </c>
+      <c r="J8" s="9">
+        <f>(C6*F8)*C32</f>
+        <v>1274.7</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10">
-        <v>2550</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="15">
+        <v>2820</v>
+      </c>
+      <c r="D9" s="16">
         <f>C9/C6</f>
-        <v>4.2009884678747937</v>
-      </c>
-      <c r="E9" s="9">
+        <v>4.6457990115321248</v>
+      </c>
+      <c r="E9" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="16">
         <f>E9/E6</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="G9" s="9">
+        <f>C9*C31</f>
+        <v>2679</v>
+      </c>
+      <c r="H9" s="13">
+        <f>C9*C32</f>
+        <v>2961</v>
+      </c>
+      <c r="I9" s="14">
+        <f>(C6*F9)*C31</f>
+        <v>2652.5899999999997</v>
+      </c>
+      <c r="J9" s="9">
+        <f>(C6*F9)*C32</f>
+        <v>2931.81</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13">
-        <v>3243</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="C10" s="15">
+        <v>2095</v>
+      </c>
+      <c r="D10" s="16">
         <f>C10/C6</f>
-        <v>5.3426688632619443</v>
-      </c>
-      <c r="E10" s="12">
+        <v>3.4514003294892914</v>
+      </c>
+      <c r="E10" s="6">
         <v>1.8</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="16">
         <f>E10/E6</f>
         <v>3.6</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="G10" s="9">
+        <f>C10*C31</f>
+        <v>1990.25</v>
+      </c>
+      <c r="H10" s="13">
+        <f>C10*C32</f>
+        <v>2199.75</v>
+      </c>
+      <c r="I10" s="14">
+        <f>(C6*F10)*C31</f>
+        <v>2075.94</v>
+      </c>
+      <c r="J10" s="9">
+        <f>(C6*F10)*C32</f>
+        <v>2294.4600000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>1.05</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
General update after AMMR work
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Lying on back</t>
   </si>
   <si>
-    <t>seating flexed no support</t>
-  </si>
-  <si>
     <t>seating relaxed</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>percent error max</t>
   </si>
   <si>
-    <t>Flexed actively foward?</t>
-  </si>
-  <si>
     <t>% min error</t>
   </si>
   <si>
@@ -109,16 +103,13 @@
   </si>
   <si>
     <t>optimal % max error</t>
-  </si>
-  <si>
-    <t>The photo shows that the elbows are resting on the legs, which is unknown forces.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,19 +132,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,29 +161,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,14 +315,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Ark1'!$B$2:$B$10</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Ark1'!$B$2,'Ark1'!$B$4:$B$10)</c:f>
+              <c:f>'Ark1'!$B$2:$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -365,40 +347,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Ark1'!$D$2:$D$10</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Ark1'!$D$2,'Ark1'!$D$4:$D$10)</c:f>
+              <c:f>'Ark1'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.24546952224052718</c:v>
+                  <c:v>0.10276679841897234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64415156507413507</c:v>
+                  <c:v>0.48418972332015808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1976935749588138</c:v>
+                  <c:v>0.89328063241106714</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1054365733113674</c:v>
+                  <c:v>2.1067193675889326</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0955518945634268</c:v>
+                  <c:v>2.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6457990115321248</c:v>
+                  <c:v>5.2173913043478262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4514003294892914</c:v>
+                  <c:v>4.1897233201581026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,14 +410,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Ark1'!$B$2:$B$10</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Ark1'!$B$2,'Ark1'!$B$4:$B$10)</c:f>
+              <c:f>'Ark1'!$B$2:$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -474,14 +442,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Ark1'!$F$2:$F$10</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Ark1'!$F$2,'Ark1'!$F$4:$F$10)</c:f>
+              <c:f>'Ark1'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1262,13 +1223,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1560,419 +1521,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="3"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="37.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="13.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>52</v>
+      </c>
+      <c r="D2" s="4">
+        <f>C2/C5</f>
+        <v>0.10276679841897234</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="4">
+        <f>E2/E5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="5">
+        <f>C2*C30</f>
+        <v>49.4</v>
+      </c>
+      <c r="H2" s="6">
+        <f>C2*C31</f>
+        <v>54.6</v>
+      </c>
+      <c r="I2" s="7">
+        <f>(C5*F2)*C30</f>
+        <v>96.14</v>
+      </c>
+      <c r="J2" s="7">
+        <f>(D5*G2)*C31</f>
+        <v>51.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>245</v>
+      </c>
+      <c r="D3" s="4">
+        <f>C3/C5</f>
+        <v>0.48418972332015808</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="F3" s="4">
+        <f>E3/E5</f>
+        <v>0.54</v>
+      </c>
+      <c r="G3" s="5">
+        <f>C3*C30</f>
+        <v>232.75</v>
+      </c>
+      <c r="H3" s="6">
+        <f>C3*C31</f>
+        <v>257.25</v>
+      </c>
+      <c r="I3" s="7">
+        <f>(C5*F3)*C30</f>
+        <v>259.57799999999997</v>
+      </c>
+      <c r="J3" s="7">
+        <f>(C5*F3)*C31</f>
+        <v>286.90200000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>452</v>
+      </c>
+      <c r="D4" s="4">
+        <f>C4/C5</f>
+        <v>0.89328063241106714</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="F4" s="4">
+        <f>E4/E5</f>
+        <v>0.9</v>
+      </c>
+      <c r="G4" s="5">
+        <f>C4*C30</f>
+        <v>429.4</v>
+      </c>
+      <c r="H4" s="6">
+        <f>C4*C31</f>
+        <v>474.6</v>
+      </c>
+      <c r="I4" s="7">
+        <f>(C5*F4)*C30</f>
+        <v>432.63</v>
+      </c>
+      <c r="J4" s="7">
+        <f>(C5*F4)*C31</f>
+        <v>478.17000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
+      <c r="C5" s="3">
+        <v>506</v>
+      </c>
+      <c r="D5" s="4">
+        <f>C5/C5</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="4">
+        <f>E5/E5</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <f>C5*C30</f>
+        <v>480.7</v>
+      </c>
+      <c r="H5" s="6">
+        <f>C5*C31</f>
+        <v>531.30000000000007</v>
+      </c>
+      <c r="I5" s="7">
+        <f>(C5*F5)*C30</f>
+        <v>480.7</v>
+      </c>
+      <c r="J5" s="7">
+        <f>(C5*F5)*C31</f>
+        <v>531.30000000000007</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>149</v>
-      </c>
-      <c r="D2" s="3">
-        <f>C2/C6</f>
-        <v>0.24546952224052718</v>
-      </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="3">
-        <f>E2/E6</f>
-        <v>0.2</v>
-      </c>
-      <c r="G2" s="9">
-        <f>C2*C31</f>
-        <v>141.54999999999998</v>
-      </c>
-      <c r="H2" s="10">
-        <f>C2*C32</f>
-        <v>156.45000000000002</v>
-      </c>
-      <c r="I2" s="14">
-        <f>(C6*F2)*C31</f>
-        <v>115.33</v>
-      </c>
-      <c r="J2" s="14">
-        <f>(D6*G2)*C32</f>
-        <v>148.6275</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1066</v>
+      </c>
+      <c r="D6" s="4">
+        <f>C6/C5</f>
+        <v>2.1067193675889326</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F6" s="4">
+        <f>E6/E5</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G6" s="5">
+        <f>C6*C30</f>
+        <v>1012.6999999999999</v>
+      </c>
+      <c r="H6" s="6">
+        <f>C6*C31</f>
+        <v>1119.3</v>
+      </c>
+      <c r="I6" s="7">
+        <f>(C5*F6)*C30</f>
+        <v>1057.54</v>
+      </c>
+      <c r="J6" s="7">
+        <f>(C5*F6)*C31</f>
+        <v>1168.8600000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1242</v>
+      </c>
+      <c r="D7" s="11">
+        <f>C7/C5</f>
+        <v>2.4545454545454546</v>
+      </c>
+      <c r="E7" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <f>C3/C6</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F3" s="5">
-        <f>E3/E6</f>
+      <c r="F7" s="11">
+        <f>E7/E5</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="5">
+        <f>C7*C30</f>
+        <v>1179.8999999999999</v>
+      </c>
+      <c r="H7" s="12">
+        <f>C7*C31</f>
+        <v>1304.1000000000001</v>
+      </c>
+      <c r="I7" s="7">
+        <f>(C5*F7)*C30</f>
+        <v>961.4</v>
+      </c>
+      <c r="J7" s="5">
+        <f>(C5*F7)*C31</f>
+        <v>1062.6000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2640</v>
+      </c>
+      <c r="D8" s="11">
+        <f>C8/C5</f>
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F8" s="11">
+        <f>E8/E5</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G8" s="5">
+        <f>C8*C30</f>
+        <v>2508</v>
+      </c>
+      <c r="H8" s="12">
+        <f>C8*C31</f>
+        <v>2772</v>
+      </c>
+      <c r="I8" s="7">
+        <f>(C5*F8)*C30</f>
+        <v>2211.2199999999998</v>
+      </c>
+      <c r="J8" s="5">
+        <f>(C5*F8)*C31</f>
+        <v>2443.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2120</v>
+      </c>
+      <c r="D9" s="11">
+        <f>C9/C5</f>
+        <v>4.1897233201581026</v>
+      </c>
+      <c r="E9" s="9">
         <v>1.8</v>
       </c>
-      <c r="G3" s="11">
-        <f>C3*C31</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="17">
-        <f>C3*C32</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="11">
-        <f>(C6*F3)*C31</f>
-        <v>1037.97</v>
-      </c>
-      <c r="J3" s="11">
-        <f>(C6*F3)*C32</f>
-        <v>1147.2300000000002</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
+      <c r="F9" s="11">
+        <f>E9/E5</f>
+        <v>3.6</v>
+      </c>
+      <c r="G9" s="5">
+        <f>C9*C30</f>
+        <v>2014</v>
+      </c>
+      <c r="H9" s="12">
+        <f>C9*C31</f>
+        <v>2226</v>
+      </c>
+      <c r="I9" s="7">
+        <f>(C5*F9)*C30</f>
+        <v>1730.52</v>
+      </c>
+      <c r="J9" s="5">
+        <f>(C5*F9)*C31</f>
+        <v>1912.6800000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>391</v>
-      </c>
-      <c r="D4" s="3">
-        <f>C4/C6</f>
-        <v>0.64415156507413507</v>
-      </c>
-      <c r="E4">
-        <v>0.27</v>
-      </c>
-      <c r="F4" s="3">
-        <f>E4/E6</f>
-        <v>0.54</v>
-      </c>
-      <c r="G4" s="9">
-        <f>C4*C31</f>
-        <v>371.45</v>
-      </c>
-      <c r="H4" s="10">
-        <f>C4*C32</f>
-        <v>410.55</v>
-      </c>
-      <c r="I4" s="14">
-        <f>(C6*F4)*C31</f>
-        <v>311.39100000000002</v>
-      </c>
-      <c r="J4" s="14">
-        <f>(C6*F4)*C32</f>
-        <v>344.16900000000004</v>
-      </c>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7">
-        <v>727</v>
-      </c>
-      <c r="D5" s="3">
-        <f>C5/C6</f>
-        <v>1.1976935749588138</v>
-      </c>
-      <c r="E5">
-        <v>0.45</v>
-      </c>
-      <c r="F5" s="3">
-        <f>E5/E6</f>
-        <v>0.9</v>
-      </c>
-      <c r="G5" s="9">
-        <f>C5*C31</f>
-        <v>690.65</v>
-      </c>
-      <c r="H5" s="10">
-        <f>C5*C32</f>
-        <v>763.35</v>
-      </c>
-      <c r="I5" s="14">
-        <f>(C6*F5)*C31</f>
-        <v>518.98500000000001</v>
-      </c>
-      <c r="J5" s="14">
-        <f>(C6*F5)*C32</f>
-        <v>573.61500000000012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>607</v>
-      </c>
-      <c r="D6" s="3">
-        <f>C6/C6</f>
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="3">
-        <f>E6/E6</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
-        <f>C6*C31</f>
-        <v>576.65</v>
-      </c>
-      <c r="H6" s="10">
-        <f>C6*C32</f>
-        <v>637.35</v>
-      </c>
-      <c r="I6" s="14">
-        <f>(C6*F6)*C31</f>
-        <v>576.65</v>
-      </c>
-      <c r="J6" s="14">
-        <f>(C6*F6)*C32</f>
-        <v>637.35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1278</v>
-      </c>
-      <c r="D7" s="3">
-        <f>C7/C6</f>
-        <v>2.1054365733113674</v>
-      </c>
-      <c r="E7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F7" s="3">
-        <f>E7/E6</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G7" s="9">
-        <f>C7*C31</f>
-        <v>1214.0999999999999</v>
-      </c>
-      <c r="H7" s="10">
-        <f>C7*C32</f>
-        <v>1341.9</v>
-      </c>
-      <c r="I7" s="14">
-        <f>(C6*F7)*C31</f>
-        <v>1268.6300000000001</v>
-      </c>
-      <c r="J7" s="14">
-        <f>(C6*F7)*C32</f>
-        <v>1402.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="15">
-        <v>1272</v>
-      </c>
-      <c r="D8" s="16">
-        <f>C8/C6</f>
-        <v>2.0955518945634268</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="16">
-        <f>E8/E6</f>
-        <v>2</v>
-      </c>
-      <c r="G8" s="9">
-        <f>C8*C31</f>
-        <v>1208.3999999999999</v>
-      </c>
-      <c r="H8" s="13">
-        <f>C8*C32</f>
-        <v>1335.6000000000001</v>
-      </c>
-      <c r="I8" s="14">
-        <f>(C6*F8)*C31</f>
-        <v>1153.3</v>
-      </c>
-      <c r="J8" s="9">
-        <f>(C6*F8)*C32</f>
-        <v>1274.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="15">
-        <v>2820</v>
-      </c>
-      <c r="D9" s="16">
-        <f>C9/C6</f>
-        <v>4.6457990115321248</v>
-      </c>
-      <c r="E9" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F9" s="16">
-        <f>E9/E6</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G9" s="9">
-        <f>C9*C31</f>
-        <v>2679</v>
-      </c>
-      <c r="H9" s="13">
-        <f>C9*C32</f>
-        <v>2961</v>
-      </c>
-      <c r="I9" s="14">
-        <f>(C6*F9)*C31</f>
-        <v>2652.5899999999997</v>
-      </c>
-      <c r="J9" s="9">
-        <f>(C6*F9)*C32</f>
-        <v>2931.81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="15">
-        <v>2095</v>
-      </c>
-      <c r="D10" s="16">
-        <f>C10/C6</f>
-        <v>3.4514003294892914</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1.8</v>
-      </c>
-      <c r="F10" s="16">
-        <f>E10/E6</f>
-        <v>3.6</v>
-      </c>
-      <c r="G10" s="9">
-        <f>C10*C31</f>
-        <v>1990.25</v>
-      </c>
-      <c r="H10" s="13">
-        <f>C10*C32</f>
-        <v>2199.75</v>
-      </c>
-      <c r="I10" s="14">
-        <f>(C6*F10)*C31</f>
-        <v>2075.94</v>
-      </c>
-      <c r="J10" s="9">
-        <f>(C6*F10)*C32</f>
-        <v>2294.4600000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+      <c r="C30" s="14">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="8">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32">
+      <c r="C31" s="3">
         <v>1.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hyper extended knee fix
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -352,7 +352,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.10276679841897234</c:v>
+                  <c:v>0.24110671936758893</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.48418972332015808</c:v>
@@ -1524,7 +1524,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,11 +1582,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.10276679841897234</v>
+        <v>0.24110671936758893</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1597,11 +1597,11 @@
       </c>
       <c r="G2" s="5">
         <f>C2*C30</f>
-        <v>49.4</v>
+        <v>115.89999999999999</v>
       </c>
       <c r="H2" s="6">
         <f>C2*C31</f>
-        <v>54.6</v>
+        <v>128.1</v>
       </c>
       <c r="I2" s="7">
         <f>(C5*F2)*C30</f>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="J2" s="7">
         <f>(D5*G2)*C31</f>
-        <v>51.87</v>
+        <v>121.69499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Wilke validation results
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -143,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -157,7 +157,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -335,28 +334,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.23975409836065573</c:v>
+                  <c:v>0.21550930189721865</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44672131147540983</c:v>
+                  <c:v>0.43838644317553876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90368852459016391</c:v>
+                  <c:v>0.86019524774359923</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5901639344262297</c:v>
+                  <c:v>2.3282372444280717</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.512295081967213</c:v>
+                  <c:v>2.0795726653158964</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5860655737704921</c:v>
+                  <c:v>4.7375207220482594</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3627049180327866</c:v>
+                  <c:v>3.7668078835881378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1507,7 +1506,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,7 +1557,7 @@
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.23975409836065573</v>
+        <v>0.21550930189721865</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1579,12 +1578,12 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13">
-        <v>218</v>
+      <c r="C3">
+        <v>238</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.44672131147540983</v>
+        <v>0.43838644317553876</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1605,12 +1604,12 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14">
-        <v>441</v>
+      <c r="C4">
+        <v>467</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.90368852459016391</v>
+        <v>0.86019524774359923</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1632,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="11">
-        <v>488</v>
+        <v>542.9</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1657,12 +1656,12 @@
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>1264</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.5901639344262297</v>
+        <v>2.3282372444280717</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1683,12 +1682,12 @@
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15">
-        <v>1226</v>
+      <c r="C7" s="14">
+        <v>1129</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.512295081967213</v>
+        <v>2.0795726653158964</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1709,12 +1708,12 @@
       <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15">
-        <v>2726</v>
+      <c r="C8" s="14">
+        <v>2572</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>5.5860655737704921</v>
+        <v>4.7375207220482594</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1735,12 +1734,12 @@
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15">
-        <v>2129</v>
+      <c r="C9" s="14">
+        <v>2045</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>4.3627049180327866</v>
+        <v>3.7668078835881378</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update wilke validation models
They needed update after spine stiffness was disabled.
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Lying on back</t>
   </si>
@@ -85,24 +85,6 @@
   </si>
   <si>
     <t>Fig 3e - held away about 60 cm</t>
-  </si>
-  <si>
-    <t>percent error min</t>
-  </si>
-  <si>
-    <t>percent error max</t>
-  </si>
-  <si>
-    <t>% min error</t>
-  </si>
-  <si>
-    <t>% max error</t>
-  </si>
-  <si>
-    <t>optimal % min error</t>
-  </si>
-  <si>
-    <t>optimal % max error</t>
   </si>
 </sst>
 </file>
@@ -161,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -170,17 +152,18 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,7 +261,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -352,28 +335,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.24110671936758893</c:v>
+                  <c:v>0.23975409836065573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48418972332015808</c:v>
+                  <c:v>0.44672131147540983</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89328063241106714</c:v>
+                  <c:v>0.90368852459016391</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1067193675889326</c:v>
+                  <c:v>2.5901639344262297</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4545454545454546</c:v>
+                  <c:v>2.512295081967213</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2173913043478262</c:v>
+                  <c:v>5.5860655737704921</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1897233201581026</c:v>
+                  <c:v>4.3627049180327866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,7 +515,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="61739680"/>
@@ -591,7 +574,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="53381760"/>
@@ -633,7 +616,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -663,7 +646,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1221,16 +1204,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>767715</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>55245</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1521,28 +1504,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="7" max="7" width="13.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="4"/>
+    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1561,32 +1544,21 @@
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>122</v>
+      <c r="C2" s="11">
+        <v>117</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.24110671936758893</v>
+        <v>0.23975409836065573</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1595,36 +1567,24 @@
         <f>E2/E5</f>
         <v>0.2</v>
       </c>
-      <c r="G2" s="5">
-        <f>C2*C30</f>
-        <v>115.89999999999999</v>
-      </c>
-      <c r="H2" s="6">
-        <f>C2*C31</f>
-        <v>128.1</v>
-      </c>
-      <c r="I2" s="7">
-        <f>(C5*F2)*C30</f>
-        <v>96.14</v>
-      </c>
-      <c r="J2" s="7">
-        <f>(D5*G2)*C31</f>
-        <v>121.69499999999999</v>
-      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
-        <v>245</v>
+      <c r="C3" s="13">
+        <v>218</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.48418972332015808</v>
+        <v>0.44672131147540983</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1633,36 +1593,24 @@
         <f>E3/E5</f>
         <v>0.54</v>
       </c>
-      <c r="G3" s="5">
-        <f>C3*C30</f>
-        <v>232.75</v>
-      </c>
-      <c r="H3" s="6">
-        <f>C3*C31</f>
-        <v>257.25</v>
-      </c>
-      <c r="I3" s="7">
-        <f>(C5*F3)*C30</f>
-        <v>259.57799999999997</v>
-      </c>
-      <c r="J3" s="7">
-        <f>(C5*F3)*C31</f>
-        <v>286.90200000000004</v>
-      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
-        <v>452</v>
+      <c r="C4" s="14">
+        <v>441</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.89328063241106714</v>
+        <v>0.90368852459016391</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1671,32 +1619,20 @@
         <f>E4/E5</f>
         <v>0.9</v>
       </c>
-      <c r="G4" s="5">
-        <f>C4*C30</f>
-        <v>429.4</v>
-      </c>
-      <c r="H4" s="6">
-        <f>C4*C31</f>
-        <v>474.6</v>
-      </c>
-      <c r="I4" s="7">
-        <f>(C5*F4)*C30</f>
-        <v>432.63</v>
-      </c>
-      <c r="J4" s="7">
-        <f>(C5*F4)*C31</f>
-        <v>478.17000000000007</v>
-      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
-        <v>506</v>
+      <c r="C5" s="11">
+        <v>488</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1709,36 +1645,24 @@
         <f>E5/E5</f>
         <v>1</v>
       </c>
-      <c r="G5" s="5">
-        <f>C5*C30</f>
-        <v>480.7</v>
-      </c>
-      <c r="H5" s="6">
-        <f>C5*C31</f>
-        <v>531.30000000000007</v>
-      </c>
-      <c r="I5" s="7">
-        <f>(C5*F5)*C30</f>
-        <v>480.7</v>
-      </c>
-      <c r="J5" s="7">
-        <f>(C5*F5)*C31</f>
-        <v>531.30000000000007</v>
-      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8">
-        <v>1066</v>
+      <c r="C6" s="14">
+        <v>1264</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.1067193675889326</v>
+        <v>2.5901639344262297</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1747,155 +1671,94 @@
         <f>E6/E5</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="G6" s="5">
-        <f>C6*C30</f>
-        <v>1012.6999999999999</v>
-      </c>
-      <c r="H6" s="6">
-        <f>C6*C31</f>
-        <v>1119.3</v>
-      </c>
-      <c r="I6" s="7">
-        <f>(C5*F6)*C30</f>
-        <v>1057.54</v>
-      </c>
-      <c r="J6" s="7">
-        <f>(C5*F6)*C31</f>
-        <v>1168.8600000000001</v>
-      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10">
-        <v>1242</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="15">
+        <v>1226</v>
+      </c>
+      <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.4545454545454546</v>
-      </c>
-      <c r="E7" s="9">
+        <v>2.512295081967213</v>
+      </c>
+      <c r="E7" s="8">
         <v>1</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f>E7/E5</f>
         <v>2</v>
       </c>
-      <c r="G7" s="5">
-        <f>C7*C30</f>
-        <v>1179.8999999999999</v>
-      </c>
-      <c r="H7" s="12">
-        <f>C7*C31</f>
-        <v>1304.1000000000001</v>
-      </c>
-      <c r="I7" s="7">
-        <f>(C5*F7)*C30</f>
-        <v>961.4</v>
-      </c>
-      <c r="J7" s="5">
-        <f>(C5*F7)*C31</f>
-        <v>1062.6000000000001</v>
-      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10">
-        <v>2640</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="15">
+        <v>2726</v>
+      </c>
+      <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>5.2173913043478262</v>
-      </c>
-      <c r="E8" s="9">
+        <v>5.5860655737704921</v>
+      </c>
+      <c r="E8" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <f>E8/E5</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="G8" s="5">
-        <f>C8*C30</f>
-        <v>2508</v>
-      </c>
-      <c r="H8" s="12">
-        <f>C8*C31</f>
-        <v>2772</v>
-      </c>
-      <c r="I8" s="7">
-        <f>(C5*F8)*C30</f>
-        <v>2211.2199999999998</v>
-      </c>
-      <c r="J8" s="5">
-        <f>(C5*F8)*C31</f>
-        <v>2443.98</v>
-      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10">
-        <v>2120</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="15">
+        <v>2129</v>
+      </c>
+      <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>4.1897233201581026</v>
-      </c>
-      <c r="E9" s="9">
+        <v>4.3627049180327866</v>
+      </c>
+      <c r="E9" s="8">
         <v>1.8</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f>E9/E5</f>
         <v>3.6</v>
       </c>
-      <c r="G9" s="5">
-        <f>C9*C30</f>
-        <v>2014</v>
-      </c>
-      <c r="H9" s="12">
-        <f>C9*C31</f>
-        <v>2226</v>
-      </c>
-      <c r="I9" s="7">
-        <f>(C5*F9)*C30</f>
-        <v>1730.52</v>
-      </c>
-      <c r="J9" s="5">
-        <f>(C5*F9)*C31</f>
-        <v>1912.6800000000003</v>
-      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="5"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="14">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1.05</v>
-      </c>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update wilke validation docs
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -24,9 +24,6 @@
     <t>Lying on back</t>
   </si>
   <si>
-    <t>seating relaxed</t>
-  </si>
-  <si>
     <t>Seating strait no support</t>
   </si>
   <si>
@@ -42,21 +39,6 @@
     <t>Wilke %</t>
   </si>
   <si>
-    <t>standing</t>
-  </si>
-  <si>
-    <t>standing flexed</t>
-  </si>
-  <si>
-    <t>standing lift close</t>
-  </si>
-  <si>
-    <t>standing lift flexed</t>
-  </si>
-  <si>
-    <t>standing lift stretched arms</t>
-  </si>
-  <si>
     <t>Position AMS</t>
   </si>
   <si>
@@ -85,6 +67,24 @@
   </si>
   <si>
     <t>Fig 3e - held away about 60 cm</t>
+  </si>
+  <si>
+    <t>Seating relaxed</t>
+  </si>
+  <si>
+    <t>Standing</t>
+  </si>
+  <si>
+    <t>Standing flexed</t>
+  </si>
+  <si>
+    <t>Standing lift close</t>
+  </si>
+  <si>
+    <t>Standing lift flexed</t>
+  </si>
+  <si>
+    <t>Standing lift stretched arms</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -163,6 +163,8 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,25 +306,25 @@
                   <c:v>Lying on back</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seating relaxed</c:v>
+                  <c:v>Seating relaxed</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Seating strait no support</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>standing</c:v>
+                  <c:v>Standing</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>standing flexed</c:v>
+                  <c:v>Standing flexed</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>standing lift close</c:v>
+                  <c:v>Standing lift close</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>standing lift flexed</c:v>
+                  <c:v>Standing lift flexed</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>standing lift stretched arms</c:v>
+                  <c:v>Standing lift stretched arms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -399,25 +401,25 @@
                   <c:v>Lying on back</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seating relaxed</c:v>
+                  <c:v>Seating relaxed</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Seating strait no support</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>standing</c:v>
+                  <c:v>Standing</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>standing flexed</c:v>
+                  <c:v>Standing flexed</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>standing lift close</c:v>
+                  <c:v>Standing lift close</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>standing lift flexed</c:v>
+                  <c:v>Standing lift flexed</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>standing lift stretched arms</c:v>
+                  <c:v>Standing lift stretched arms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -650,8 +652,8 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="1" l="1" r="1" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1209,10 +1211,10 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>767715</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>55245</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1506,7 +1508,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,28 +1528,28 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1573,10 +1575,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="C3">
         <v>238</v>
@@ -1599,10 +1601,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>467</v>
@@ -1625,10 +1627,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="11">
         <v>542.9</v>
@@ -1651,10 +1653,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="13">
         <v>1264</v>
@@ -1677,10 +1679,10 @@
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="C7" s="14">
         <v>1129</v>
@@ -1703,10 +1705,10 @@
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="C8" s="14">
         <v>2572</v>
@@ -1729,10 +1731,10 @@
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="C9" s="14">
         <v>2045</v>
@@ -1761,7 +1763,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Wilke Spine Pressure validation examples
The now include the TLEM2 lower extremity model. All Validation output is also updated
as well the automated tests.
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -336,28 +336,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.21550930189721865</c:v>
+                  <c:v>0.18512049938388966</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43838644317553876</c:v>
+                  <c:v>0.5567201850878748</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.86019524774359923</c:v>
+                  <c:v>0.95547766377694443</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3282372444280717</c:v>
+                  <c:v>2.3070771771936345</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0795726653158964</c:v>
+                  <c:v>2.1005175400380094</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7375207220482594</c:v>
+                  <c:v>4.7891597566936825</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7668078835881378</c:v>
+                  <c:v>3.8013963701999436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,7 +1508,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,11 +1555,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>117</v>
+        <v>101.0018</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.21550930189721865</v>
+        <v>0.18512049938388966</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1581,11 +1581,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>238</v>
+        <v>303.74669999999998</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.43838644317553876</v>
+        <v>0.5567201850878748</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1607,11 +1607,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>467</v>
+        <v>521.30889999999999</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.86019524774359923</v>
+        <v>0.95547766377694443</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1633,7 +1633,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>542.9</v>
+        <v>545.60029999999995</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1659,11 +1659,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1264</v>
+        <v>1258.742</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.3282372444280717</v>
+        <v>2.3070771771936345</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1685,11 +1685,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1129</v>
+        <v>1146.0429999999999</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0795726653158964</v>
+        <v>2.1005175400380094</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1711,11 +1711,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2572</v>
+        <v>2612.9670000000001</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.7375207220482594</v>
+        <v>4.7891597566936825</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1737,11 +1737,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>2045</v>
+        <v>2074.0430000000001</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.7668078835881378</v>
+        <v>3.8013963701999436</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update Wilke validation values
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5574A6F8-2AB3-4A7A-BBAE-E44C278CE097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -90,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -262,7 +268,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -336,28 +342,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.18512049938388966</c:v>
+                  <c:v>0.18411499953512037</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5567201850878748</c:v>
+                  <c:v>0.54697990982593714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95547766377694443</c:v>
+                  <c:v>0.93971077472327968</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3070771771936345</c:v>
+                  <c:v>2.2907272785801625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1005175400380094</c:v>
+                  <c:v>2.1277046868680398</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7891597566936825</c:v>
+                  <c:v>4.7406304271551578</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8013963701999436</c:v>
+                  <c:v>3.8180538393573764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,7 +522,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="61739680"/>
@@ -575,7 +581,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="53381760"/>
@@ -617,7 +623,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -647,7 +653,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1504,29 +1510,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="4"/>
-    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="3"/>
+    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="13.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1547,7 +1553,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1555,11 +1561,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>101.0018</v>
+        <v>102.37860000000001</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.18512049938388966</v>
+        <v>0.18411499953512037</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1573,7 +1579,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1581,11 +1587,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>303.74669999999998</v>
+        <v>304.15249999999997</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.5567201850878748</v>
+        <v>0.54697990982593714</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1599,7 +1605,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1607,11 +1613,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>521.30889999999999</v>
+        <v>522.53359999999998</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.95547766377694443</v>
+        <v>0.93971077472327968</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1625,7 +1631,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>545.60029999999995</v>
+        <v>556.05790000000002</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1651,7 +1657,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1659,11 +1665,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1258.742</v>
+        <v>1273.777</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.3070771771936345</v>
+        <v>2.2907272785801625</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1677,7 +1683,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1685,11 +1691,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1146.0429999999999</v>
+        <v>1183.127</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.1005175400380094</v>
+        <v>2.1277046868680398</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1703,7 +1709,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1711,11 +1717,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2612.9670000000001</v>
+        <v>2636.0650000000001</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.7891597566936825</v>
+        <v>4.7406304271551578</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1729,7 +1735,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1737,11 +1743,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>2074.0430000000001</v>
+        <v>2123.0590000000002</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.8013963701999436</v>
+        <v>3.8180538393573764</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>
@@ -1755,10 +1761,10 @@
       <c r="I9" s="7"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update validation results for Wilke models.
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5574A6F8-2AB3-4A7A-BBAE-E44C278CE097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB494CA-9745-40ED-8BD5-D823FFBD0B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -268,7 +271,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -342,28 +345,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.18411499953512037</c:v>
+                  <c:v>0.2015799749661219</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54697990982593714</c:v>
+                  <c:v>0.49170311822680207</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.93971077472327968</c:v>
+                  <c:v>0.89180244845882073</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2907272785801625</c:v>
+                  <c:v>2.2690198093443192</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1277046868680398</c:v>
+                  <c:v>2.0804308915174605</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7406304271551578</c:v>
+                  <c:v>4.6142014157790268</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8180538393573764</c:v>
+                  <c:v>3.6229455421725913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,7 +525,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="61739680"/>
@@ -581,7 +584,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="53381760"/>
@@ -623,7 +626,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -653,7 +656,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1514,25 +1517,25 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="7" max="7" width="13.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="4"/>
+    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1553,7 +1556,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1561,11 +1564,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>102.37860000000001</v>
+        <v>109.1407</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.18411499953512037</v>
+        <v>0.2015799749661219</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1579,7 +1582,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1587,11 +1590,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>304.15249999999997</v>
+        <v>266.221</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.54697990982593714</v>
+        <v>0.49170311822680207</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1605,7 +1608,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1613,11 +1616,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>522.53359999999998</v>
+        <v>482.84530000000001</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.93971077472327968</v>
+        <v>0.89180244845882073</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1631,7 +1634,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>556.05790000000002</v>
+        <v>541.42629999999997</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1657,7 +1660,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1665,11 +1668,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1273.777</v>
+        <v>1228.5070000000001</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.2907272785801625</v>
+        <v>2.2690198093443192</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1683,7 +1686,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1691,11 +1694,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1183.127</v>
+        <v>1126.4000000000001</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.1277046868680398</v>
+        <v>2.0804308915174605</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1709,7 +1712,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1717,11 +1720,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2636.0650000000001</v>
+        <v>2498.25</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.7406304271551578</v>
+        <v>4.6142014157790268</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1735,7 +1738,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1743,11 +1746,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>2123.0590000000002</v>
+        <v>1961.558</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.8180538393573764</v>
+        <v>3.6229455421725913</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>
@@ -1761,10 +1764,10 @@
       <c r="I9" s="7"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve implementation of internal/external obliques and latissimus dorsi muscles.
This improves the strength for trunk external rotation.

More branches are added to the internal obliques and the geometry is update to better match anatomical text books.
Likewise, the latissimus dorsi muscles is discretized into more branches so it has branch inserting on every vertebra.
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB494CA-9745-40ED-8BD5-D823FFBD0B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE01D2B-F50A-4EC4-9A38-B8F9B294FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -345,28 +345,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.2015799749661219</c:v>
+                  <c:v>0.18722851600289681</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49170311822680207</c:v>
+                  <c:v>0.50284059933615199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89180244845882073</c:v>
+                  <c:v>0.85835230788257166</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2690198093443192</c:v>
+                  <c:v>2.1124383026102964</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0804308915174605</c:v>
+                  <c:v>2.0587509470071943</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6142014157790268</c:v>
+                  <c:v>4.3880255127538437</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6229455421725913</c:v>
+                  <c:v>3.5012214211197668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1517,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,11 +1564,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>109.1407</v>
+        <v>99.767129999999995</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.2015799749661219</v>
+        <v>0.18722851600289681</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1590,11 +1590,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>266.221</v>
+        <v>267.94510000000002</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.49170311822680207</v>
+        <v>0.50284059933615199</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1616,11 +1616,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>482.84530000000001</v>
+        <v>457.38409999999999</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.89180244845882073</v>
+        <v>0.85835230788257166</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1642,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>541.42629999999997</v>
+        <v>532.86289999999997</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1668,11 +1668,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1228.5070000000001</v>
+        <v>1125.6400000000001</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.2690198093443192</v>
+        <v>2.1124383026102964</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1694,11 +1694,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1126.4000000000001</v>
+        <v>1097.0319999999999</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0804308915174605</v>
+        <v>2.0587509470071943</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1720,11 +1720,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2498.25</v>
+        <v>2338.2159999999999</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.6142014157790268</v>
+        <v>4.3880255127538437</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1746,11 +1746,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>1961.558</v>
+        <v>1865.671</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.6229455421725913</v>
+        <v>3.5012214211197668</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Improve muscles for trunk rotation (#584)
Improve implementation of internal/external obliques and latissimus dorsi muscles.

This improves the strength for trunk external rotation. More branches are added to the internal obliques and the geometry is update to better match anatomical text books. Likewise, the latissimus dorsi muscles is discretized into more branches so it has branch inserting on every vertebra.
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB494CA-9745-40ED-8BD5-D823FFBD0B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE01D2B-F50A-4EC4-9A38-B8F9B294FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -345,28 +345,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.2015799749661219</c:v>
+                  <c:v>0.18722851600289681</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49170311822680207</c:v>
+                  <c:v>0.50284059933615199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89180244845882073</c:v>
+                  <c:v>0.85835230788257166</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2690198093443192</c:v>
+                  <c:v>2.1124383026102964</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0804308915174605</c:v>
+                  <c:v>2.0587509470071943</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6142014157790268</c:v>
+                  <c:v>4.3880255127538437</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6229455421725913</c:v>
+                  <c:v>3.5012214211197668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1517,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,11 +1564,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>109.1407</v>
+        <v>99.767129999999995</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.2015799749661219</v>
+        <v>0.18722851600289681</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1590,11 +1590,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>266.221</v>
+        <v>267.94510000000002</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.49170311822680207</v>
+        <v>0.50284059933615199</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1616,11 +1616,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>482.84530000000001</v>
+        <v>457.38409999999999</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.89180244845882073</v>
+        <v>0.85835230788257166</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1642,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>541.42629999999997</v>
+        <v>532.86289999999997</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1668,11 +1668,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1228.5070000000001</v>
+        <v>1125.6400000000001</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.2690198093443192</v>
+        <v>2.1124383026102964</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1694,11 +1694,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1126.4000000000001</v>
+        <v>1097.0319999999999</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0804308915174605</v>
+        <v>2.0587509470071943</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1720,11 +1720,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2498.25</v>
+        <v>2338.2159999999999</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.6142014157790268</v>
+        <v>4.3880255127538437</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1746,11 +1746,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>1961.558</v>
+        <v>1865.671</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.6229455421725913</v>
+        <v>3.5012214211197668</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update validation study and tests after fixing transversus symmetry
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE01D2B-F50A-4EC4-9A38-B8F9B294FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F66B2-29B5-450A-83AB-A0B387378276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-225" yWindow="-16305" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -345,28 +345,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.18722851600289681</c:v>
+                  <c:v>0.15021393385724499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50284059933615199</c:v>
+                  <c:v>0.42557272056784756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85835230788257166</c:v>
+                  <c:v>0.85894944461839884</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1124383026102964</c:v>
+                  <c:v>2.0967490999927856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0587509470071943</c:v>
+                  <c:v>2.0908963986005928</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3880255127538437</c:v>
+                  <c:v>4.3559355142553038</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5012214211197668</c:v>
+                  <c:v>3.7270698283302974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1517,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,11 +1564,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>99.767129999999995</v>
+        <v>99.737080000000006</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.18722851600289681</v>
+        <v>0.15021393385724499</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1590,11 +1590,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>267.94510000000002</v>
+        <v>282.56619999999998</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.50284059933615199</v>
+        <v>0.42557272056784756</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1616,11 +1616,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>457.38409999999999</v>
+        <v>570.31399999999996</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.85835230788257166</v>
+        <v>0.85894944461839884</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1642,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>532.86289999999997</v>
+        <v>663.96690000000001</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1668,11 +1668,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1125.6400000000001</v>
+        <v>1392.172</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.1124383026102964</v>
+        <v>2.0967490999927856</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1694,11 +1694,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1097.0319999999999</v>
+        <v>1388.2860000000001</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0587509470071943</v>
+        <v>2.0908963986005928</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1720,11 +1720,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2338.2159999999999</v>
+        <v>2892.1970000000001</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.3880255127538437</v>
+        <v>4.3559355142553038</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1746,11 +1746,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>1865.671</v>
+        <v>2474.6509999999998</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.5012214211197668</v>
+        <v>3.7270698283302974</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update validation study and tests after fixing transversus symmetry (#626)
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE01D2B-F50A-4EC4-9A38-B8F9B294FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F66B2-29B5-450A-83AB-A0B387378276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-225" yWindow="-16305" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -345,28 +345,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.18722851600289681</c:v>
+                  <c:v>0.15021393385724499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50284059933615199</c:v>
+                  <c:v>0.42557272056784756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85835230788257166</c:v>
+                  <c:v>0.85894944461839884</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1124383026102964</c:v>
+                  <c:v>2.0967490999927856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0587509470071943</c:v>
+                  <c:v>2.0908963986005928</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3880255127538437</c:v>
+                  <c:v>4.3559355142553038</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5012214211197668</c:v>
+                  <c:v>3.7270698283302974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1517,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,11 +1564,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="11">
-        <v>99.767129999999995</v>
+        <v>99.737080000000006</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.18722851600289681</v>
+        <v>0.15021393385724499</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1590,11 +1590,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>267.94510000000002</v>
+        <v>282.56619999999998</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.50284059933615199</v>
+        <v>0.42557272056784756</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1616,11 +1616,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>457.38409999999999</v>
+        <v>570.31399999999996</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.85835230788257166</v>
+        <v>0.85894944461839884</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1642,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="11">
-        <v>532.86289999999997</v>
+        <v>663.96690000000001</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1668,11 +1668,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1125.6400000000001</v>
+        <v>1392.172</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.1124383026102964</v>
+        <v>2.0967490999927856</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1694,11 +1694,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1097.0319999999999</v>
+        <v>1388.2860000000001</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0587509470071943</v>
+        <v>2.0908963986005928</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1720,11 +1720,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2338.2159999999999</v>
+        <v>2892.1970000000001</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.3880255127538437</v>
+        <v>4.3559355142553038</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1746,11 +1746,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>1865.671</v>
+        <v>2474.6509999999998</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.5012214211197668</v>
+        <v>3.7270698283302974</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update Wilke validation test to accomedate new pelvis tilt
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F66B2-29B5-450A-83AB-A0B387378276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4661F5B-BD4E-4C79-B5C9-BE750E5CE832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-225" yWindow="-16305" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="-17385" windowWidth="21600" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -174,6 +174,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,28 +346,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.15021393385724499</c:v>
+                  <c:v>0.18028842105370602</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42557272056784756</c:v>
+                  <c:v>0.50881320576542699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85894944461839884</c:v>
+                  <c:v>0.89340880437665371</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0967490999927856</c:v>
+                  <c:v>2.1591805495518166</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0908963986005928</c:v>
+                  <c:v>2.0257571898995645</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3559355142553038</c:v>
+                  <c:v>4.9657374324228467</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7270698283302974</c:v>
+                  <c:v>3.7052515863055886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1518,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,12 +1564,12 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11">
-        <v>99.737080000000006</v>
+      <c r="C2">
+        <v>105.9786</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.15021393385724499</v>
+        <v>0.18028842105370602</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1590,11 +1591,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>282.56619999999998</v>
+        <v>299.09469999999999</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.42557272056784756</v>
+        <v>0.50881320576542699</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1616,11 +1617,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>570.31399999999996</v>
+        <v>525.17079999999999</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.85894944461839884</v>
+        <v>0.89340880437665371</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1641,8 +1642,8 @@
       <c r="B5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="11">
-        <v>663.96690000000001</v>
+      <c r="C5" s="17">
+        <v>587.82809999999995</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1668,11 +1669,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1392.172</v>
+        <v>1269.2270000000001</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.0967490999927856</v>
+        <v>2.1591805495518166</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1694,11 +1695,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1388.2860000000001</v>
+        <v>1190.797</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0908963986005928</v>
+        <v>2.0257571898995645</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1720,11 +1721,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2892.1970000000001</v>
+        <v>2919</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.3559355142553038</v>
+        <v>4.9657374324228467</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1746,11 +1747,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>2474.6509999999998</v>
+        <v>2178.0509999999999</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.7270698283302974</v>
+        <v>3.7052515863055886</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update wilke test results
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A569E8-F46E-4831-8EA0-D4353BAFF4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4E15D-ECBA-4BAC-9363-3AAAC1301088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7980" yWindow="-15720" windowWidth="21600" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,28 +346,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.21896655662926115</c:v>
+                  <c:v>0.20730606720226763</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59922810199199283</c:v>
+                  <c:v>0.56731778173488889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89563890047007477</c:v>
+                  <c:v>0.84794400089224686</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2917885863355538</c:v>
+                  <c:v>2.1697453985938009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1132330782177826</c:v>
+                  <c:v>2.0699537412529847</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9551172001547483</c:v>
+                  <c:v>4.6912454353913944</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8639738122060776</c:v>
+                  <c:v>3.6582080255170442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.21896655662926115</v>
+        <v>0.20730606720226763</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.59922810199199283</v>
+        <v>0.56731778173488889</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.89563890047007477</v>
+        <v>0.84794400089224686</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1643,7 +1643,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="17">
-        <v>499.13330000000002</v>
+        <v>527.20839999999998</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.2917885863355538</v>
+        <v>2.1697453985938009</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1695,11 +1695,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1054.7850000000001</v>
+        <v>1091.297</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.1132330782177826</v>
+        <v>2.0699537412529847</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.9551172001547483</v>
+        <v>4.6912454353913944</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.8639738122060776</v>
+        <v>3.6582080255170442</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update wilke trend validation
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4E15D-ECBA-4BAC-9363-3AAAC1301088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AFAA1E-A1F7-401A-9CCC-E24097F08FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="-15720" windowWidth="21600" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5535" yWindow="4215" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -346,28 +346,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.20730606720226763</c:v>
+                  <c:v>0.20347226633400894</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56731778173488889</c:v>
+                  <c:v>0.55449254304702456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84794400089224686</c:v>
+                  <c:v>0.82494367184318118</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1697453985938009</c:v>
+                  <c:v>2.1101489255436339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0699537412529847</c:v>
+                  <c:v>2.0547540110291624</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6912454353913944</c:v>
+                  <c:v>4.5121847282414427</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6582080255170442</c:v>
+                  <c:v>3.6352999390945966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,11 +1565,11 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>109.29349999999999</v>
+        <v>114.3553</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.20730606720226763</v>
+        <v>0.20347226633400894</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1591,11 +1591,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>299.09469999999999</v>
+        <v>311.6354</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.56731778173488889</v>
+        <v>0.55449254304702456</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1617,11 +1617,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>447.04320000000001</v>
+        <v>463.63409999999999</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.84794400089224686</v>
+        <v>0.82494367184318118</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1643,7 +1643,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="17">
-        <v>527.20839999999998</v>
+        <v>562.01909999999998</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1669,11 +1669,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1143.9079999999999</v>
+        <v>1185.944</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.1697453985938009</v>
+        <v>2.1101489255436339</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1695,11 +1695,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1091.297</v>
+        <v>1154.8109999999999</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0699537412529847</v>
+        <v>2.0547540110291624</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1721,11 +1721,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2473.2640000000001</v>
+        <v>2535.9340000000002</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.6912454353913944</v>
+        <v>4.5121847282414427</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1747,11 +1747,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>1928.6379999999999</v>
+        <v>2043.1079999999999</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.6582080255170442</v>
+        <v>3.6352999390945966</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Adjust psoas via points and origins (#731)
* Adjust psoas via points and origins

This is a followup to HS's adjustments which solves the problem with erector spinae (sacrum-L5) beeing
overloaded when trunk carries an extension moment.

* Update wilke trend validation
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED4E15D-ECBA-4BAC-9363-3AAAC1301088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AFAA1E-A1F7-401A-9CCC-E24097F08FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="-15720" windowWidth="21600" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5535" yWindow="4215" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -346,28 +346,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.20730606720226763</c:v>
+                  <c:v>0.20347226633400894</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56731778173488889</c:v>
+                  <c:v>0.55449254304702456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84794400089224686</c:v>
+                  <c:v>0.82494367184318118</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1697453985938009</c:v>
+                  <c:v>2.1101489255436339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0699537412529847</c:v>
+                  <c:v>2.0547540110291624</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6912454353913944</c:v>
+                  <c:v>4.5121847282414427</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6582080255170442</c:v>
+                  <c:v>3.6352999390945966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,11 +1565,11 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>109.29349999999999</v>
+        <v>114.3553</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.20730606720226763</v>
+        <v>0.20347226633400894</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1591,11 +1591,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>299.09469999999999</v>
+        <v>311.6354</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.56731778173488889</v>
+        <v>0.55449254304702456</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1617,11 +1617,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>447.04320000000001</v>
+        <v>463.63409999999999</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.84794400089224686</v>
+        <v>0.82494367184318118</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1643,7 +1643,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="17">
-        <v>527.20839999999998</v>
+        <v>562.01909999999998</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1669,11 +1669,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1143.9079999999999</v>
+        <v>1185.944</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.1697453985938009</v>
+        <v>2.1101489255436339</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1695,11 +1695,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1091.297</v>
+        <v>1154.8109999999999</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0699537412529847</v>
+        <v>2.0547540110291624</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1721,11 +1721,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2473.2640000000001</v>
+        <v>2535.9340000000002</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.6912454353913944</v>
+        <v>4.5121847282414427</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1747,11 +1747,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>1928.6379999999999</v>
+        <v>2043.1079999999999</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.6582080255170442</v>
+        <v>3.6352999390945966</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Update Wilke reference tests (#742)
* Add support script for running and updating wilke files

* Fix test which could not run kinematically

* Update wilke validation results
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AFAA1E-A1F7-401A-9CCC-E24097F08FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023DEFF7-2EEC-43CE-875A-9CBA28132954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="4215" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2730" yWindow="-16305" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -346,28 +346,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.20347226633400894</c:v>
+                  <c:v>0.19117899433670843</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55449254304702456</c:v>
+                  <c:v>0.52445512270465078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82494367184318118</c:v>
+                  <c:v>0.81036553972884839</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1101489255436339</c:v>
+                  <c:v>2.0882100566329154</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0547540110291624</c:v>
+                  <c:v>2.1403809850695041</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5121847282414427</c:v>
+                  <c:v>4.3391110348378241</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6352999390945966</c:v>
+                  <c:v>3.7055088381671522</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,11 +1565,11 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>114.3553</v>
+        <v>111.4</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.20347226633400894</v>
+        <v>0.19117899433670843</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1591,11 +1591,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>311.6354</v>
+        <v>305.60000000000002</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.55449254304702456</v>
+        <v>0.52445512270465078</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1617,11 +1617,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>463.63409999999999</v>
+        <v>472.2</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.82494367184318118</v>
+        <v>0.81036553972884839</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1643,7 +1643,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="17">
-        <v>562.01909999999998</v>
+        <v>582.70000000000005</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1669,11 +1669,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="13">
-        <v>1185.944</v>
+        <v>1216.8</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.1101489255436339</v>
+        <v>2.0882100566329154</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1695,11 +1695,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="14">
-        <v>1154.8109999999999</v>
+        <v>1247.2</v>
       </c>
       <c r="D7" s="9">
         <f>C7/C5</f>
-        <v>2.0547540110291624</v>
+        <v>2.1403809850695041</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -1721,11 +1721,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="14">
-        <v>2535.9340000000002</v>
+        <v>2528.4</v>
       </c>
       <c r="D8" s="9">
         <f>C8/C5</f>
-        <v>4.5121847282414427</v>
+        <v>4.3391110348378241</v>
       </c>
       <c r="E8" s="8">
         <v>2.2999999999999998</v>
@@ -1747,11 +1747,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="14">
-        <v>2043.1079999999999</v>
+        <v>2159.1999999999998</v>
       </c>
       <c r="D9" s="9">
         <f>C9/C5</f>
-        <v>3.6352999390945966</v>
+        <v>3.7055088381671522</v>
       </c>
       <c r="E9" s="8">
         <v>1.8</v>

</xml_diff>

<commit_message>
Updated from newest excel sheet with muscle parameters (#761)
* Updated from newest excel sheet with muscle parameters

* Pectoralis_minor changed from 4 to 3 muscle elements.
The muscle connected to R2 is removed since there is no Pectoralis minor connected to R2.
The naming was started from top to down, and we needed to remove the old Pectoralis_minor_1. So the cyl also moved from old Pectoralis_minor_2 to new Pectoralis_minor_1.

* Lumbar Semispinalis is removed since there is no equivalent in anatomy.

* Solve failed tests, except SpinePressures

* Update wilke tests

* Update CHANGELOG.md

---------

Co-authored-by: hs <hs@anybodytech.com>
Co-authored-by: Morten Enemark Lund <mel@anybodytech.com>
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A569E8-F46E-4831-8EA0-D4353BAFF4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B44354-DE75-4832-98CC-33D97B2E1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="-15720" windowWidth="21600" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -152,16 +152,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -169,12 +167,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,28 +339,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.21896655662926115</c:v>
+                  <c:v>0.17925591882750846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59922810199199283</c:v>
+                  <c:v>0.4620711869866323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89563890047007477</c:v>
+                  <c:v>0.78611692704139158</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2917885863355538</c:v>
+                  <c:v>2.0479948461910129</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1132330782177826</c:v>
+                  <c:v>2.1468835561282011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9551172001547483</c:v>
+                  <c:v>4.1451119342889351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8639738122060776</c:v>
+                  <c:v>3.8144628764696411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,7 +1511,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,11 +1558,11 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>109.29349999999999</v>
+        <v>111.3</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.21896655662926115</v>
+        <v>0.17925591882750846</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1580,22 +1573,22 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3">
-        <v>299.09469999999999</v>
+        <v>286.89999999999998</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.59922810199199283</v>
+        <v>0.4620711869866323</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1606,8 +1599,8 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1617,11 +1610,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>447.04320000000001</v>
+        <v>488.1</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.89563890047007477</v>
+        <v>0.78611692704139158</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1632,18 +1625,18 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="17">
-        <v>499.13330000000002</v>
+      <c r="C5" s="12">
+        <v>620.9</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1658,22 +1651,22 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13">
-        <v>1143.9079999999999</v>
+      <c r="C6" s="11">
+        <v>1271.5999999999999</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.2917885863355538</v>
+        <v>2.0479948461910129</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1684,92 +1677,92 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="14">
-        <v>1054.7850000000001</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C7" s="11">
+        <v>1333</v>
+      </c>
+      <c r="D7" s="7">
         <f>C7/C5</f>
-        <v>2.1132330782177826</v>
-      </c>
-      <c r="E7" s="8">
+        <v>2.1468835561282011</v>
+      </c>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <f>E7/E5</f>
         <v>2</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="14">
-        <v>2473.2640000000001</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="C8" s="11">
+        <v>2573.6999999999998</v>
+      </c>
+      <c r="D8" s="7">
         <f>C8/C5</f>
-        <v>4.9551172001547483</v>
-      </c>
-      <c r="E8" s="8">
+        <v>4.1451119342889351</v>
+      </c>
+      <c r="E8" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <f>E8/E5</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="14">
-        <v>1928.6379999999999</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="C9" s="11">
+        <v>2368.4</v>
+      </c>
+      <c r="D9" s="7">
         <f>C9/C5</f>
-        <v>3.8639738122060776</v>
-      </c>
-      <c r="E9" s="8">
+        <v>3.8144628764696411</v>
+      </c>
+      <c r="E9" s="3">
         <v>1.8</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <f>E9/E5</f>
         <v>3.6</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="12"/>
+      <c r="C30" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add AMMR 3.0 Thoracic model development
This commit adds all current development on the AMMR 3.0 detailed
thoracic model plus the new volume based abdominal model.

Co-authored-by: Hamed Shayestehpour <hs@anybodytech.com>
Co-authored-by: Bjørn Keller Engelund <bke@anybodytech.com>
Co-authored-by: Pavel E. Galibarov <peg@anybodytech.com>
Co-authored-by: Søren Tørholm <st@anybodytech.com>
Co-authored-by: Michael Damsgaard <md@anybodytech.com>
</commit_message>
<xml_diff>
--- a/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
+++ b/Application/Validation/WilkeSpinalDiscPressure/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B44354-DE75-4832-98CC-33D97B2E1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E78079-BDED-47A3-8F69-0BDE4ACA6D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2910" yWindow="-19650" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -339,28 +339,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.17925591882750846</c:v>
+                  <c:v>0.25499412455934195</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4620711869866323</c:v>
+                  <c:v>0.48329696155783103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78611692704139158</c:v>
+                  <c:v>0.76817189860668122</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0479948461910129</c:v>
+                  <c:v>2.1534329360416313</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1468835561282011</c:v>
+                  <c:v>1.9833808964243744</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1451119342889351</c:v>
+                  <c:v>4.7228470706731578</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8144628764696411</c:v>
+                  <c:v>3.5551452073191205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1511,7 +1511,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,11 +1558,11 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>111.3</v>
+        <v>151.9</v>
       </c>
       <c r="D2" s="4">
         <f>C2/C5</f>
-        <v>0.17925591882750846</v>
+        <v>0.25499412455934195</v>
       </c>
       <c r="E2" s="3">
         <v>0.1</v>
@@ -1584,11 +1584,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>286.89999999999998</v>
+        <v>287.89999999999998</v>
       </c>
       <c r="D3" s="4">
         <f>C3/C5</f>
-        <v>0.4620711869866323</v>
+        <v>0.48329696155783103</v>
       </c>
       <c r="E3" s="3">
         <v>0.27</v>
@@ -1610,11 +1610,11 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>488.1</v>
+        <v>457.6</v>
       </c>
       <c r="D4" s="4">
         <f>C4/C5</f>
-        <v>0.78611692704139158</v>
+        <v>0.76817189860668122</v>
       </c>
       <c r="E4" s="3">
         <v>0.45</v>
@@ -1636,7 +1636,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="12">
-        <v>620.9</v>
+        <v>595.70000000000005</v>
       </c>
       <c r="D5" s="4">
         <f>C5/C5</f>
@@ -1662,11 +1662,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="11">
-        <v>1271.5999999999999</v>
+        <v>1282.8</v>
       </c>
       <c r="D6" s="4">
         <f>C6/C5</f>
-        <v>2.0479948461910129</v>
+        <v>2.1534329360416313</v>
       </c>
       <c r="E6" s="3">
         <v>1.1000000000000001</v>
@@ -1688,11 +1688,11 @@
         <v>19</v>
       </c>
       <c r="C7" s="11">
-        <v>1333</v>
+        <v>1181.5</v>
       </c>
       <c r="D7" s="7">
         <f>C7/C5</f>
-        <v>2.1468835561282011</v>
+        <v>1.9833808964243744</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1714,11 +1714,11 @@
         <v>20</v>
       </c>
       <c r="C8" s="11">
-        <v>2573.6999999999998</v>
+        <v>2813.4</v>
       </c>
       <c r="D8" s="7">
         <f>C8/C5</f>
-        <v>4.1451119342889351</v>
+        <v>4.7228470706731578</v>
       </c>
       <c r="E8" s="3">
         <v>2.2999999999999998</v>
@@ -1740,11 +1740,11 @@
         <v>21</v>
       </c>
       <c r="C9" s="11">
-        <v>2368.4</v>
+        <v>2117.8000000000002</v>
       </c>
       <c r="D9" s="7">
         <f>C9/C5</f>
-        <v>3.8144628764696411</v>
+        <v>3.5551452073191205</v>
       </c>
       <c r="E9" s="3">
         <v>1.8</v>

</xml_diff>